<commit_message>
Bug fixes in Visione
</commit_message>
<xml_diff>
--- a/Query per popolare il DB/Visione.xlsx
+++ b/Query per popolare il DB/Visione.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caste\Desktop\2ndYear\db\ProgettoBasiDiDati\Query per popolare il DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABBBDBC-EEA1-4729-B836-81403D68512B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADC1BCA-99CA-4ECA-869F-F8FC7317ABED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CDE8A788-FB39-418F-89E5-1F8BEB6F86AE}"/>
   </bookViews>
@@ -477,10 +477,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -798,12 +797,12 @@
   <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -813,7 +812,7 @@
       <c r="A1" t="s">
         <v>135</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>134</v>
       </c>
       <c r="C1" t="s">
@@ -830,7 +829,7 @@
       <c r="A2">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C2" t="s">
@@ -847,7 +846,7 @@
       <c r="A3">
         <v>20</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C3" t="s">
@@ -864,7 +863,7 @@
       <c r="A4">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C4" t="s">
@@ -881,7 +880,7 @@
       <c r="A5">
         <v>30</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C5" t="s">
@@ -898,7 +897,7 @@
       <c r="A6">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C6" t="s">
@@ -915,7 +914,7 @@
       <c r="A7">
         <v>20</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C7" t="s">
@@ -932,7 +931,7 @@
       <c r="A8">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C8" t="s">
@@ -949,7 +948,7 @@
       <c r="A9">
         <v>20</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C9" t="s">
@@ -966,7 +965,7 @@
       <c r="A10">
         <v>20</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C10" t="s">
@@ -983,41 +982,41 @@
       <c r="A11">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
+      <c r="B11" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>20</v>
+      <c r="B12" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E12" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>20</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C13" t="s">
@@ -1027,48 +1026,48 @@
         <v>110</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>20</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>112</v>
+      <c r="B14" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E14" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>20</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>112</v>
+      <c r="B15" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>20</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C16" t="s">
@@ -1078,167 +1077,167 @@
         <v>106</v>
       </c>
       <c r="E16" t="s">
-        <v>109</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>20</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>108</v>
+      <c r="B17" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>20</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>108</v>
+      <c r="B18" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>20</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="E19" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>20</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>15</v>
+      <c r="B21" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>0</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>15</v>
+      <c r="B22" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>102</v>
+      <c r="B23" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>20</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>97</v>
+      <c r="B24" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>20</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>97</v>
+      <c r="B25" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>20</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C26" t="s">
@@ -1248,82 +1247,82 @@
         <v>90</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>20</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>92</v>
+      <c r="B27" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E27" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>20</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>92</v>
+      <c r="B28" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E28" t="s">
-        <v>0</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>20</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>88</v>
+      <c r="B29" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E29" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>20</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>88</v>
+      <c r="B30" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>20</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C31" t="s">
@@ -1333,653 +1332,653 @@
         <v>80</v>
       </c>
       <c r="E31" t="s">
-        <v>84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>20</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>82</v>
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E32" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>20</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>82</v>
+        <v>30</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E33" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>20</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>78</v>
+        <v>30</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>20</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>78</v>
+        <v>30</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="E35" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>30</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>74</v>
+        <v>15</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="E36" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>30</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>74</v>
+        <v>15</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E37" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
+        <v>15</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" t="s">
         <v>30</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E38" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>30</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>70</v>
+        <v>15</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="E39" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>30</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>63</v>
+        <v>15</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="E40" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
+        <v>15</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" t="s">
         <v>30</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" t="s">
-        <v>62</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E41" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>30</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>63</v>
+        <v>20</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="E42" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>30</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>63</v>
+        <v>20</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="E43" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>30</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>63</v>
+        <v>15</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="E44" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>30</v>
-      </c>
-      <c r="B45" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B45" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C45" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="E45" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>30</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>54</v>
+        <v>20</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="E46" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>30</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>54</v>
+        <v>15</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="E47" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>30</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>54</v>
+        <v>15</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="E48" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>30</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>49</v>
+        <v>20</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>30</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>49</v>
+        <v>20</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>15</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>46</v>
+        <v>20</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>15</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>42</v>
+        <v>20</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>15</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>15</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>15</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="C55" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="E55" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>15</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="E56" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>15</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="C57" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="E57" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>15</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="C58" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="E58" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>15</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="C59" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="E59" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
+        <v>20</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C60" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="E60" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>20</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>20</v>
+      <c r="B61" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>19</v>
+        <v>104</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
       <c r="E61" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>20</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C62" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="E62" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>20</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C63" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="E63" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>20</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="E64" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>20</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>10</v>
+      <c r="B65" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C65" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E65" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>20</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>3</v>
+      <c r="B66" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C66" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E66" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>20</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C67" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="E67" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>20</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C68" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="E68" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>20</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C69" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="E69" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>